<commit_message>
Product backlog e Api Arq Comp
</commit_message>
<xml_diff>
--- a/Documentação/planoDeAção BackLog PlanilhaDeRiscos.xlsx
+++ b/Documentação/planoDeAção BackLog PlanilhaDeRiscos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPRINT2\MushRoomCompany\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a176d51d6e478c2b/Área de Trabalho/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB880CDE-D282-4D26-9735-BCF4682302FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAC166A4-04B5-4BD9-BCB1-46D92DBE0869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>Estruturar e montar o circuito do Arduino, junto ao script para os sensores</t>
   </si>
   <si>
-    <t>Tela para o site institucional onde o usuário vai poder fazer seu cadastro. Todos os campos da página devem estar preenchidos corretamente</t>
-  </si>
-  <si>
     <t>Projetos atualizado no GitHub</t>
   </si>
   <si>
@@ -469,9 +466,6 @@
     <t>Todas</t>
   </si>
   <si>
-    <t>Sistema de Cadastro</t>
-  </si>
-  <si>
     <t>Sistema de login</t>
   </si>
   <si>
@@ -515,6 +509,12 @@
   </si>
   <si>
     <t>R11</t>
+  </si>
+  <si>
+    <t>Não  Funcional</t>
+  </si>
+  <si>
+    <t>Sistema o qual será computado o cadastro</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1028,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1174,6 +1174,87 @@
     <xf numFmtId="0" fontId="11" fillId="32" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1196,45 +1277,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1265,49 +1307,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1624,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="64" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1646,49 +1652,49 @@
   <sheetData>
     <row r="1" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="51"/>
+      <c r="B1" s="76" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="78"/>
     </row>
     <row r="2" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="G2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>54</v>
-      </c>
       <c r="I2" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -1700,10 +1706,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" s="16">
         <v>8</v>
@@ -1712,15 +1718,15 @@
         <v>1</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -1729,10 +1735,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="16">
         <v>8</v>
@@ -1741,12 +1747,12 @@
         <v>6</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -1758,10 +1764,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="17">
         <v>5</v>
@@ -1770,15 +1776,15 @@
         <v>9</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -1786,11 +1792,11 @@
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="19">
         <v>13</v>
@@ -1799,53 +1805,53 @@
         <v>8</v>
       </c>
       <c r="I6" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="83" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="80">
+        <v>8</v>
+      </c>
+      <c r="H7" s="79">
+        <v>4</v>
+      </c>
+      <c r="I7" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="M6" s="8"/>
-    </row>
-    <row r="7" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="55" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="53">
-        <v>8</v>
-      </c>
-      <c r="H7" s="52">
-        <v>4</v>
-      </c>
-      <c r="I7" s="61" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="8" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="85"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="62"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="67"/>
     </row>
     <row r="9" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -1857,10 +1863,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="17">
         <v>5</v>
@@ -1869,27 +1875,27 @@
         <v>3</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10" s="16">
         <v>8</v>
@@ -1898,27 +1904,27 @@
         <v>5</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="18">
         <v>3</v>
@@ -1927,27 +1933,27 @@
         <v>10</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="17">
         <v>5</v>
@@ -1956,27 +1962,27 @@
         <v>12</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="19">
         <v>13</v>
@@ -1985,27 +1991,27 @@
         <v>7</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G14" s="17">
         <v>5</v>
@@ -2014,27 +2020,27 @@
         <v>13</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G15" s="18">
         <v>3</v>
@@ -2043,27 +2049,27 @@
         <v>14</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>42</v>
+      <c r="A16" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G16" s="18">
         <v>3</v>
@@ -2072,27 +2078,27 @@
         <v>11</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="50" t="s">
         <v>55</v>
-      </c>
-      <c r="C17" s="82" t="s">
-        <v>56</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" s="16">
         <v>8</v>
@@ -2101,27 +2107,27 @@
         <v>2</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="52" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" s="16">
         <v>8</v>
@@ -2130,27 +2136,27 @@
         <v>15</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="C19" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="52" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G19" s="17">
         <v>5</v>
@@ -2159,27 +2165,27 @@
         <v>16</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="D20" s="86" t="s">
+      <c r="D20" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>28</v>
+      <c r="E20" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G20" s="17">
         <v>5</v>
@@ -2188,27 +2194,27 @@
         <v>17</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C21" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" s="86" t="s">
+      <c r="D21" s="52" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G21" s="17">
         <v>5</v>
@@ -2217,27 +2223,27 @@
         <v>18</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="D22" s="86" t="s">
+      <c r="D22" s="52" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G22" s="16">
         <v>8</v>
@@ -2245,28 +2251,28 @@
       <c r="H22" s="20">
         <v>19</v>
       </c>
-      <c r="I22" s="87" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D23" s="86" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G23" s="17">
         <v>5</v>
@@ -2275,27 +2281,27 @@
         <v>20</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D24" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>154</v>
       </c>
       <c r="G24" s="17">
         <v>5</v>
@@ -2304,27 +2310,27 @@
         <v>21</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D25" s="86" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="52" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G25" s="17">
         <v>5</v>
@@ -2333,28 +2339,29 @@
         <v>22</v>
       </c>
       <c r="I25" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="83"/>
-    </row>
-    <row r="32" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-    </row>
-    <row r="33" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="51"/>
+    </row>
+    <row r="32" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="96" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="96"/>
+      <c r="C32" s="96"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="96"/>
+      <c r="G32" s="96"/>
+      <c r="H32" s="96"/>
+      <c r="I32" s="96"/>
+      <c r="J32" s="96"/>
+    </row>
+    <row r="33" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
@@ -2366,10 +2373,10 @@
         <v>2</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G33" s="17">
         <v>5</v>
@@ -2378,139 +2385,105 @@
         <v>9</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="84" t="s">
+        <v>59</v>
+      </c>
+      <c r="J33" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="59" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="59" t="s">
+      <c r="B34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="17">
+        <v>5</v>
+      </c>
+      <c r="H34" s="20">
+        <v>3</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J34" s="21"/>
+    </row>
+    <row r="35" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="17">
+        <v>5</v>
+      </c>
+      <c r="H35" s="20">
+        <v>12</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J35" s="21"/>
+    </row>
+    <row r="36" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="16">
         <v>8</v>
       </c>
-      <c r="D34" s="57" t="s">
+      <c r="H36" s="20">
         <v>2</v>
       </c>
-      <c r="E34" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="G34" s="66">
-        <v>8</v>
-      </c>
-      <c r="H34" s="64">
-        <v>4</v>
-      </c>
-      <c r="I34" s="61" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="85"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="62"/>
-    </row>
-    <row r="36" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" s="17">
-        <v>5</v>
-      </c>
-      <c r="H36" s="20">
-        <v>3</v>
-      </c>
       <c r="I36" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G37" s="17">
-        <v>5</v>
-      </c>
-      <c r="H37" s="20">
-        <v>12</v>
-      </c>
-      <c r="I37" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="82" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G38" s="16">
-        <v>8</v>
-      </c>
-      <c r="H38" s="20">
-        <v>2</v>
-      </c>
-      <c r="I38" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="J36" s="21"/>
+    </row>
+    <row r="44" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B44" s="38"/>
       <c r="C44" s="38"/>
@@ -2521,9 +2494,9 @@
       <c r="H44" s="38"/>
       <c r="I44" s="38"/>
     </row>
-    <row r="45" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="88" t="s">
-        <v>33</v>
+    <row r="45" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="54" t="s">
+        <v>32</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>0</v>
@@ -2535,27 +2508,27 @@
         <v>2</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" s="89" t="s">
-        <v>49</v>
-      </c>
-      <c r="G45" s="89">
+        <v>26</v>
+      </c>
+      <c r="F45" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="G45" s="55">
         <v>8</v>
       </c>
-      <c r="H45" s="90">
-        <v>1</v>
-      </c>
-      <c r="I45" s="91" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="88" t="s">
-        <v>34</v>
+      <c r="H45" s="56">
+        <v>2</v>
+      </c>
+      <c r="I45" s="57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="54" t="s">
+        <v>33</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
@@ -2564,27 +2537,27 @@
         <v>2</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F46" s="89" t="s">
-        <v>49</v>
-      </c>
-      <c r="G46" s="89">
+        <v>26</v>
+      </c>
+      <c r="F46" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" s="55">
         <v>8</v>
       </c>
-      <c r="H46" s="90">
-        <v>6</v>
-      </c>
-      <c r="I46" s="91" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="92" t="s">
-        <v>36</v>
+      <c r="H46" s="56">
+        <v>3</v>
+      </c>
+      <c r="I46" s="57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="58" t="s">
+        <v>35</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>6</v>
@@ -2592,431 +2565,472 @@
       <c r="D47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F47" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" s="59">
+        <v>13</v>
+      </c>
+      <c r="H47" s="56">
+        <v>8</v>
+      </c>
+      <c r="I47" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="F47" s="93" t="s">
+      <c r="F48" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="G47" s="93">
-        <v>13</v>
-      </c>
-      <c r="H47" s="90">
+      <c r="G48" s="70">
         <v>8</v>
       </c>
-      <c r="I47" s="91" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="88" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="H48" s="68">
         <v>7</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F48" s="89" t="s">
-        <v>49</v>
-      </c>
-      <c r="G48" s="89">
-        <v>8</v>
-      </c>
-      <c r="H48" s="90">
-        <v>5</v>
-      </c>
-      <c r="I48" s="91" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="92" t="s">
-        <v>40</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F49" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="G49" s="94">
-        <v>3</v>
-      </c>
-      <c r="H49" s="90">
-        <v>10</v>
-      </c>
-      <c r="I49" s="91" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="88" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>16</v>
+      <c r="I48" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="J48" s="49"/>
+    </row>
+    <row r="49" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="75"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="73"/>
+      <c r="F49" s="71"/>
+      <c r="G49" s="71"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="97"/>
+      <c r="J49" s="98"/>
+    </row>
+    <row r="50" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>17</v>
+        <v>161</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F50" s="93" t="s">
+      <c r="F50" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="G50" s="93">
+      <c r="G50" s="55">
+        <v>8</v>
+      </c>
+      <c r="H50" s="56">
+        <v>5</v>
+      </c>
+      <c r="I50" s="57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="G51" s="60">
+        <v>3</v>
+      </c>
+      <c r="H51" s="56">
+        <v>11</v>
+      </c>
+      <c r="I51" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="G52" s="59">
         <v>13</v>
       </c>
-      <c r="H50" s="90">
+      <c r="H52" s="56">
+        <v>6</v>
+      </c>
+      <c r="I52" s="57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="91" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="88" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" s="26" t="s">
+      <c r="E53" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F53" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="G53" s="55">
+        <v>8</v>
+      </c>
+      <c r="H53" s="56">
+        <v>10</v>
+      </c>
+      <c r="I53" s="57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="D51" s="86" t="s">
+      <c r="B54" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E54" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F51" s="89" t="s">
+      <c r="F54" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="G54" s="55">
+        <v>8</v>
+      </c>
+      <c r="H54" s="56">
+        <v>9</v>
+      </c>
+      <c r="I54" s="57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="G51" s="89">
+      <c r="G55" s="61">
+        <v>3</v>
+      </c>
+      <c r="H55" s="56">
+        <v>7</v>
+      </c>
+      <c r="I55" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="G56" s="60">
+        <v>3</v>
+      </c>
+      <c r="H56" s="56">
+        <v>13</v>
+      </c>
+      <c r="I56" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="G57" s="60">
+        <v>3</v>
+      </c>
+      <c r="H57" s="56">
+        <v>14</v>
+      </c>
+      <c r="I57" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D58" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="G58" s="61">
         <v>5</v>
       </c>
-      <c r="H51" s="90">
+      <c r="H58" s="56">
+        <v>15</v>
+      </c>
+      <c r="I58" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D59" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="G59" s="61">
+        <v>5</v>
+      </c>
+      <c r="H59" s="56">
+        <v>4</v>
+      </c>
+      <c r="I59" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="D60" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="G60" s="55">
         <v>8</v>
       </c>
-      <c r="I51" s="91" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="88" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="5" t="s">
+      <c r="H60" s="56">
+        <v>1</v>
+      </c>
+      <c r="I60" s="57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D61" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F52" s="89" t="s">
+      <c r="F61" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="G52" s="89">
+      <c r="G61" s="61">
         <v>5</v>
       </c>
-      <c r="H52" s="90">
-        <v>8</v>
-      </c>
-      <c r="I52" s="91" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="88" t="s">
-        <v>158</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D53" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" s="5" t="s">
+      <c r="H61" s="56">
+        <v>16</v>
+      </c>
+      <c r="I61" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D62" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F53" s="95" t="s">
-        <v>50</v>
-      </c>
-      <c r="G53" s="95">
-        <v>3</v>
-      </c>
-      <c r="H53" s="90"/>
-      <c r="I53" s="91" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="92" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F54" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="G54" s="94">
-        <v>3</v>
-      </c>
-      <c r="H54" s="90">
-        <v>14</v>
-      </c>
-      <c r="I54" s="91" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="88" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F55" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="G55" s="94">
-        <v>3</v>
-      </c>
-      <c r="H55" s="90">
-        <v>11</v>
-      </c>
-      <c r="I55" s="91" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="88" t="s">
-        <v>134</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C56" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56" s="95" t="s">
-        <v>50</v>
-      </c>
-      <c r="G56" s="95">
+      <c r="F62" s="61" t="s">
+        <v>152</v>
+      </c>
+      <c r="G62" s="61">
         <v>5</v>
       </c>
-      <c r="H56" s="90"/>
-      <c r="I56" s="91" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="88" t="s">
-        <v>68</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="D57" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F57" s="95" t="s">
-        <v>50</v>
-      </c>
-      <c r="G57" s="95">
+      <c r="H62" s="56">
+        <v>17</v>
+      </c>
+      <c r="I62" s="57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D63" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F63" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="G63" s="61">
         <v>5</v>
       </c>
-      <c r="H57" s="90"/>
-      <c r="I57" s="91" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="92" t="s">
-        <v>142</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="D58" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F58" s="89" t="s">
-        <v>49</v>
-      </c>
-      <c r="G58" s="89">
-        <v>8</v>
-      </c>
-      <c r="H58" s="90"/>
-      <c r="I58" s="91" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="88" t="s">
-        <v>148</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D59" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F59" s="95" t="s">
-        <v>50</v>
-      </c>
-      <c r="G59" s="95">
-        <v>5</v>
-      </c>
-      <c r="H59" s="90"/>
-      <c r="I59" s="91" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="88" t="s">
-        <v>151</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D60" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F60" s="95" t="s">
-        <v>154</v>
-      </c>
-      <c r="G60" s="95">
-        <v>5</v>
-      </c>
-      <c r="H60" s="90"/>
-      <c r="I60" s="91" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="88" t="s">
-        <v>155</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D61" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F61" s="95" t="s">
-        <v>50</v>
-      </c>
-      <c r="G61" s="95">
-        <v>5</v>
-      </c>
-      <c r="H61" s="90"/>
-      <c r="I61" s="91" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="96"/>
+      <c r="H63" s="56">
+        <v>18</v>
+      </c>
+      <c r="I63" s="57" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A34:A35"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G7:G8"/>
@@ -3025,6 +3039,18 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A32:J32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3052,71 +3078,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="A1" s="84" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="72"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
+      <c r="A3" s="86"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
+      <c r="A4" s="88"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="C5" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="D5" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="E5" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="F5" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="H5" s="34" t="s">
         <v>80</v>
-      </c>
-      <c r="H5" s="34" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3124,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="31">
         <v>2</v>
@@ -3136,13 +3162,13 @@
         <v>2</v>
       </c>
       <c r="F6" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="H6" s="24" t="s">
         <v>84</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3150,7 +3176,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="31">
         <v>3</v>
@@ -3162,13 +3188,13 @@
         <v>3</v>
       </c>
       <c r="F7" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="24" t="s">
         <v>88</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3176,7 +3202,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="31">
         <v>2</v>
@@ -3188,13 +3214,13 @@
         <v>4</v>
       </c>
       <c r="F8" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="24" t="s">
         <v>91</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3202,7 +3228,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="31">
         <v>1</v>
@@ -3214,13 +3240,13 @@
         <v>4</v>
       </c>
       <c r="F9" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>96</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3228,7 +3254,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="10">
         <v>2</v>
@@ -3240,13 +3266,13 @@
         <v>2</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3254,7 +3280,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="31">
         <v>1</v>
@@ -3266,13 +3292,13 @@
         <v>3</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3280,7 +3306,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="31">
         <v>1</v>
@@ -3292,13 +3318,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3306,7 +3332,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C13" s="31">
         <v>2</v>
@@ -3318,13 +3344,13 @@
         <v>2</v>
       </c>
       <c r="F13" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="37" t="s">
         <v>106</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="H13" s="37" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="17" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3356,133 +3382,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="69" x14ac:dyDescent="1.1499999999999999">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="90" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="92"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="93" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="78"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="81"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="95"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="39" t="s">
+      <c r="D3" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="E3" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="F3" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="39" t="s">
         <v>113</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="C4" s="40" t="s">
         <v>116</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>117</v>
       </c>
       <c r="D4" s="41">
         <v>45208</v>
       </c>
       <c r="E4" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="40" t="s">
         <v>118</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>119</v>
       </c>
       <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:7" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="42" t="s">
         <v>120</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>121</v>
       </c>
       <c r="D5" s="43">
         <v>45208</v>
       </c>
       <c r="E5" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="G5" s="42" t="s">
         <v>123</v>
-      </c>
-      <c r="G5" s="42" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D6" s="46">
         <v>45208</v>
       </c>
       <c r="E6" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="47" t="s">
         <v>126</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>127</v>
       </c>
       <c r="G6" s="45"/>
     </row>
     <row r="7" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="43">
         <v>45208</v>
       </c>
       <c r="E7" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="42" t="s">
         <v>129</v>
-      </c>
-      <c r="F7" s="42" t="s">
-        <v>130</v>
       </c>
       <c r="G7" s="42"/>
     </row>

</xml_diff>